<commit_message>
layout and nav for tech home page
</commit_message>
<xml_diff>
--- a/Docs/Excel/OnSiteXI.xlsx
+++ b/Docs/Excel/OnSiteXI.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\_A\_UX\OnSiteXI\Docs\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\_A\_UX\OnSiteX\Docs\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12795" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12795" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="App Component" sheetId="1" r:id="rId1"/>
     <sheet name="UserConfig" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="HomePage HTML" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="208">
   <si>
     <t>declarations:[</t>
   </si>
@@ -436,57 +436,6 @@
     <t>pyrlClass</t>
   </si>
   <si>
-    <t>Number of Assignments: 11</t>
-  </si>
-  <si>
-    <t>HALLIBURTON BROWNFIELD PMPSHOP M-TECH</t>
-  </si>
-  <si>
-    <t>HALLIBURTON BROWNFIELD MAIN E-TECH</t>
-  </si>
-  <si>
-    <t>HALLIBURTON ODESSA BASE MAIN E-TECH</t>
-  </si>
-  <si>
-    <t>HALLIBURTON ODESSA BASE MAIN M-TECH</t>
-  </si>
-  <si>
-    <t>HALLIBURTON ODESSA BASE MAIN TOPPER</t>
-  </si>
-  <si>
-    <t>KEANE SHAWNEE MAIN M-TECH</t>
-  </si>
-  <si>
-    <t>KEANE SPRINGTOWN MAIN E-TECH</t>
-  </si>
-  <si>
-    <t>KEANE SPRINGTOWN MAIN M-TECH</t>
-  </si>
-  <si>
-    <t>SESA WESLACO SHOP M-TECH</t>
-  </si>
-  <si>
-    <t>SESA WESLACO OFFICE ADMIN</t>
-  </si>
-  <si>
-    <t>SESA LAS CUATAS MAIN M-TECH</t>
-  </si>
-  <si>
-    <t>;</t>
-  </si>
-  <si>
-    <t>settings.ts:36</t>
-  </si>
-  <si>
-    <t>ionViewDidLoad SettingsPage</t>
-  </si>
-  <si>
-    <t>settings.ts:37</t>
-  </si>
-  <si>
-    <t>settings.ts:45</t>
-  </si>
-  <si>
     <t>clntCmpny = [</t>
   </si>
   <si>
@@ -575,16 +524,139 @@
   </si>
   <si>
     <t>PYRLCLASS</t>
+  </si>
+  <si>
+    <t>&lt;ion-icon name="</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t>Open Work Orders</t>
+  </si>
+  <si>
+    <t>calendar</t>
+  </si>
+  <si>
+    <t>clock</t>
+  </si>
+  <si>
+    <t>Shift Info</t>
+  </si>
+  <si>
+    <t>cloud-upload</t>
+  </si>
+  <si>
+    <t>Upload Reports</t>
+  </si>
+  <si>
+    <t>&lt;/ion-note&gt;</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Calendar View</t>
+  </si>
+  <si>
+    <t>Upload</t>
+  </si>
+  <si>
+    <t>Create New Work Order</t>
+  </si>
+  <si>
+    <t>settings</t>
+  </si>
+  <si>
+    <t>User/Report Settings</t>
+  </si>
+  <si>
+    <t>&lt;button ion-item</t>
+  </si>
+  <si>
+    <t>(click)="newReport()"&gt;</t>
+  </si>
+  <si>
+    <t>(click)="openReports()"&gt;</t>
+  </si>
+  <si>
+    <t>(click)="viewCalendar()"&gt;</t>
+  </si>
+  <si>
+    <t>(click)="shiftsPage()"&gt;</t>
+  </si>
+  <si>
+    <t>(click)="uploadReports()"&gt;</t>
+  </si>
+  <si>
+    <t>(click)="settings()"&gt;</t>
+  </si>
+  <si>
+    <t>" color="secondary"&gt;&lt;/ion-icon&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> icon-left color="Primary"</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>" color="primary"&gt;&lt;/ion-icon&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/ion-list-header&gt;</t>
+  </si>
+  <si>
+    <t>{{today}}</t>
+  </si>
+  <si>
+    <t>Schedule/Past Reports</t>
+  </si>
+  <si>
+    <t>Complete Shift:</t>
+  </si>
+  <si>
+    <t>&lt;ion-list-header color="med-dark"&gt;</t>
+  </si>
+  <si>
+    <t>Report: Technician Information</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ion-note item-right</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> color="splash"&gt;</t>
+  </si>
+  <si>
+    <t>" color="favorite"&gt;&lt;/ion-icon&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> color="secondary"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> color="light"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> color="favorite"&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-  </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -618,6 +690,11 @@
       <color rgb="FF000000"/>
       <name val="Roboto Mono Light"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Roboto Condensed Light"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -639,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -656,7 +733,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1580,7 +1658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+    <sheetView topLeftCell="D4" workbookViewId="0">
       <selection activeCell="H25" sqref="H25:H29"/>
     </sheetView>
   </sheetViews>
@@ -2101,13 +2179,13 @@
         <v>49</v>
       </c>
       <c r="H25" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="I25" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="J25" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="K25" t="s">
         <v>116</v>
@@ -2121,25 +2199,25 @@
         <v>49</v>
       </c>
       <c r="H26" t="s">
+        <v>137</v>
+      </c>
+      <c r="I26" t="s">
+        <v>151</v>
+      </c>
+      <c r="J26" t="s">
+        <v>152</v>
+      </c>
+      <c r="K26" t="s">
+        <v>153</v>
+      </c>
+      <c r="L26" t="s">
         <v>154</v>
       </c>
-      <c r="I26" t="s">
-        <v>168</v>
-      </c>
-      <c r="J26" t="s">
-        <v>169</v>
-      </c>
-      <c r="K26" t="s">
-        <v>170</v>
-      </c>
-      <c r="L26" t="s">
-        <v>171</v>
-      </c>
       <c r="M26" s="9" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="N26" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="O26" t="s">
         <v>15</v>
@@ -2159,19 +2237,19 @@
         <v>49</v>
       </c>
       <c r="H27" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="I27" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="J27" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="K27" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="L27" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="M27" t="s">
         <v>15</v>
@@ -2185,19 +2263,19 @@
         <v>49</v>
       </c>
       <c r="H28" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="I28" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="J28" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="K28" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="L28" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="M28" t="s">
         <v>15</v>
@@ -2211,31 +2289,31 @@
         <v>49</v>
       </c>
       <c r="H29" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="I29" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="J29" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="K29" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="L29" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="M29" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="N29" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="O29" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="P29" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="Q29" t="s">
         <v>2</v>
@@ -2267,7 +2345,7 @@
         <v>75</v>
       </c>
       <c r="E34" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="H34" t="s">
         <v>70</v>
@@ -2285,7 +2363,7 @@
         <v>50</v>
       </c>
       <c r="M34" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -2293,7 +2371,7 @@
         <v>76</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="H35" t="s">
         <v>58</v>
@@ -2304,7 +2382,7 @@
         <v>77</v>
       </c>
       <c r="E36" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="H36" t="s">
         <v>64</v>
@@ -2315,7 +2393,7 @@
         <v>78</v>
       </c>
       <c r="E37" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H37" t="s">
         <v>50</v>
@@ -2326,10 +2404,10 @@
         <v>79</v>
       </c>
       <c r="E38" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="H38" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -2337,7 +2415,7 @@
         <v>80</v>
       </c>
       <c r="E39" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
@@ -2345,7 +2423,7 @@
         <v>81</v>
       </c>
       <c r="E40" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
@@ -2353,7 +2431,7 @@
         <v>82</v>
       </c>
       <c r="E41" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -2536,204 +2614,316 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F12:J24"/>
+  <dimension ref="B6:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:K24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="A6:Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="17.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.625" customWidth="1"/>
+    <col min="1" max="2" width="9" style="10"/>
+    <col min="3" max="3" width="22.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.75" style="10" customWidth="1"/>
+    <col min="5" max="5" width="22.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" style="10" customWidth="1"/>
+    <col min="14" max="14" width="15.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="12" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F12" s="10">
-        <v>42733.693697118055</v>
-      </c>
-      <c r="H12" t="s">
-        <v>150</v>
-      </c>
-      <c r="I12" t="s">
-        <v>148</v>
-      </c>
-      <c r="J12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F13" s="10">
-        <v>42733.693697199073</v>
-      </c>
-      <c r="H13" t="s">
-        <v>136</v>
-      </c>
-      <c r="I13" t="s">
-        <v>148</v>
-      </c>
-      <c r="J13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F14" s="10">
-        <v>42733.693697210649</v>
-      </c>
-      <c r="H14" t="s">
-        <v>137</v>
-      </c>
-      <c r="I14" t="s">
-        <v>148</v>
-      </c>
-      <c r="J14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F15" s="10">
-        <v>42733.693697233794</v>
-      </c>
-      <c r="H15" t="s">
-        <v>138</v>
-      </c>
-      <c r="I15" t="s">
-        <v>148</v>
-      </c>
-      <c r="J15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F16" s="10">
-        <v>42733.693697256946</v>
-      </c>
-      <c r="H16" t="s">
-        <v>139</v>
-      </c>
-      <c r="I16" t="s">
-        <v>148</v>
-      </c>
-      <c r="J16" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F17" s="10">
-        <v>42733.69369728009</v>
-      </c>
-      <c r="H17" t="s">
-        <v>140</v>
-      </c>
-      <c r="I17" t="s">
-        <v>148</v>
-      </c>
-      <c r="J17" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F18" s="10">
-        <v>42733.693697303243</v>
-      </c>
-      <c r="H18" t="s">
-        <v>141</v>
-      </c>
-      <c r="I18" t="s">
-        <v>148</v>
-      </c>
-      <c r="J18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F19" s="10">
-        <v>42733.693697314811</v>
-      </c>
-      <c r="H19" t="s">
-        <v>142</v>
-      </c>
-      <c r="I19" t="s">
-        <v>148</v>
-      </c>
-      <c r="J19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F20" s="10">
-        <v>42733.693697326387</v>
-      </c>
-      <c r="H20" t="s">
-        <v>143</v>
-      </c>
-      <c r="I20" t="s">
-        <v>148</v>
-      </c>
-      <c r="J20" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F21" s="10">
-        <v>42733.693697349539</v>
-      </c>
-      <c r="H21" t="s">
-        <v>144</v>
-      </c>
-      <c r="I21" t="s">
-        <v>148</v>
-      </c>
-      <c r="J21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F22" s="10">
-        <v>42733.693697361108</v>
-      </c>
-      <c r="H22" t="s">
-        <v>145</v>
-      </c>
-      <c r="I22" t="s">
-        <v>148</v>
-      </c>
-      <c r="J22" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F23" s="10">
-        <v>42733.693697372684</v>
-      </c>
-      <c r="H23" t="s">
-        <v>146</v>
-      </c>
-      <c r="I23" t="s">
-        <v>148</v>
-      </c>
-      <c r="J23" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F24" s="10">
-        <v>42733.69369738426</v>
-      </c>
-      <c r="H24" t="s">
-        <v>147</v>
-      </c>
-      <c r="I24" t="s">
-        <v>148</v>
-      </c>
-      <c r="J24" t="s">
-        <v>152</v>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C6" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="E7" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="E8" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="E10" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B11" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="E12" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="E13" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="E15" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>